<commit_message>
cleaning up the Roxygen comments within the full wing function
</commit_message>
<xml_diff>
--- a/data/Master_AnatomicalData.xlsx
+++ b/data/Master_AnatomicalData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E89F270-AA11-4BA3-B2A9-060E340EA221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE82F6DF-98AB-493B-A37D-A4BD6772F66D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33300" yWindow="2055" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="6" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="4500" yWindow="2055" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="6" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -52,9 +52,6 @@
     <t>lar_gla</t>
   </si>
   <si>
-    <t>Feather</t>
-  </si>
-  <si>
     <t>vane_angle</t>
   </si>
   <si>
@@ -928,9 +925,6 @@
     <t>l_vane</t>
   </si>
   <si>
-    <t>w_r</t>
-  </si>
-  <si>
     <t>w_vp</t>
   </si>
   <si>
@@ -962,6 +956,12 @@
   </si>
   <si>
     <t>m_f</t>
+  </si>
+  <si>
+    <t>feather</t>
+  </si>
+  <si>
+    <t>w_cal</t>
   </si>
 </sst>
 </file>
@@ -8401,19 +8401,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
         <v>57</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -8421,84 +8421,84 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" t="s">
-        <v>55</v>
-      </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" t="s">
-        <v>55</v>
-      </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -8544,60 +8544,60 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>178</v>
-      </c>
       <c r="G1" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="9" t="s">
-        <v>235</v>
-      </c>
       <c r="I1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>191</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>154</v>
-      </c>
       <c r="M1" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="N1" s="13" t="s">
         <v>243</v>
       </c>
-      <c r="N1" s="13" t="s">
-        <v>244</v>
-      </c>
       <c r="O1" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E2">
         <v>0.14599999999999999</v>
@@ -8615,13 +8615,13 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="J2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2">
         <v>1995</v>
       </c>
       <c r="L2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M2" s="14">
         <f>0.00194*E2^1.953</f>
@@ -8638,16 +8638,16 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3">
         <v>2.14</v>
@@ -8665,7 +8665,7 @@
         <v>0.216</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K3">
         <v>1995</v>
@@ -8685,16 +8685,16 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E4">
         <v>0.56899999999999995</v>
@@ -8712,7 +8712,7 @@
         <v>0.108</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K4">
         <v>1995</v>
@@ -8732,16 +8732,16 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E5">
         <v>0.27900000000000003</v>
@@ -8759,7 +8759,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="J5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K5">
         <v>1995</v>
@@ -8779,16 +8779,16 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6">
         <v>0.77100000000000002</v>
@@ -8806,7 +8806,7 @@
         <v>0.155</v>
       </c>
       <c r="J6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K6">
         <v>1995</v>
@@ -8826,16 +8826,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7">
         <v>1.374E-2</v>
@@ -8850,7 +8850,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="J7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K7">
         <v>1995</v>
@@ -8870,16 +8870,16 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8">
         <v>0.39300000000000002</v>
@@ -8897,7 +8897,7 @@
         <v>0.06</v>
       </c>
       <c r="J8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K8">
         <v>1995</v>
@@ -8917,16 +8917,16 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E9">
         <v>0.13200000000000001</v>
@@ -8944,7 +8944,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="J9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K9">
         <v>1995</v>
@@ -8964,16 +8964,16 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10">
         <v>0.36399999999999999</v>
@@ -8991,7 +8991,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K10">
         <v>1995</v>
@@ -9011,16 +9011,16 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E11">
         <v>0.16300000000000001</v>
@@ -9038,7 +9038,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="J11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K11">
         <v>1995</v>
@@ -9058,16 +9058,16 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E12">
         <v>0.25600000000000001</v>
@@ -9085,7 +9085,7 @@
         <v>0.11799999999999999</v>
       </c>
       <c r="J12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K12">
         <v>1995</v>
@@ -9105,16 +9105,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E13">
         <v>0.1</v>
@@ -9132,7 +9132,7 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="J13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K13">
         <v>1995</v>
@@ -9152,16 +9152,16 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E14">
         <v>0.69099999999999995</v>
@@ -9179,7 +9179,7 @@
         <v>0.1</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K14">
         <v>1995</v>
@@ -9199,16 +9199,16 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E15">
         <v>0.29299999999999998</v>
@@ -9226,7 +9226,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K15">
         <v>1995</v>
@@ -9246,16 +9246,16 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E16">
         <v>0.39800000000000002</v>
@@ -9273,7 +9273,7 @@
         <v>0.111</v>
       </c>
       <c r="J16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K16">
         <v>1995</v>
@@ -9293,16 +9293,16 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E17">
         <v>3.4299999999999997E-2</v>
@@ -9320,7 +9320,7 @@
         <v>0.03</v>
       </c>
       <c r="J17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K17">
         <v>1995</v>
@@ -9340,16 +9340,16 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E18">
         <v>0.17899999999999999</v>
@@ -9367,7 +9367,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="J18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K18">
         <v>1995</v>
@@ -9387,16 +9387,16 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19">
         <v>6.2899999999999998E-2</v>
@@ -9414,7 +9414,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="J19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K19">
         <v>1995</v>
@@ -9434,16 +9434,16 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20">
         <v>1.52E-2</v>
@@ -9461,7 +9461,7 @@
         <v>0.03</v>
       </c>
       <c r="J20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K20">
         <v>1995</v>
@@ -9481,16 +9481,16 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E21">
         <v>1.4999999999999999E-2</v>
@@ -9508,7 +9508,7 @@
         <v>2.1999999999999999E-2</v>
       </c>
       <c r="J21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K21">
         <v>1995</v>
@@ -9528,16 +9528,16 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E22">
         <v>5.62E-2</v>
@@ -9555,7 +9555,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
       <c r="J22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K22">
         <v>1995</v>
@@ -9575,16 +9575,16 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E23">
         <v>6.7599999999999993E-2</v>
@@ -9602,7 +9602,7 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="J23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K23">
         <v>1995</v>
@@ -9622,16 +9622,16 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E24">
         <v>1.46E-2</v>
@@ -9649,7 +9649,7 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="J24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K24">
         <v>1995</v>
@@ -9669,16 +9669,16 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E25">
         <v>9.4999999999999998E-3</v>
@@ -9696,7 +9696,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="J25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K25">
         <v>1995</v>
@@ -9716,16 +9716,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E26">
         <v>1.9900000000000001E-2</v>
@@ -9743,7 +9743,7 @@
         <v>2.3E-2</v>
       </c>
       <c r="J26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K26">
         <v>1995</v>
@@ -9763,16 +9763,16 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E27">
         <v>1.4500000000000001E-2</v>
@@ -9790,7 +9790,7 @@
         <v>1.9E-2</v>
       </c>
       <c r="J27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27">
         <v>1995</v>
@@ -9810,16 +9810,16 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E28">
         <v>1.5100000000000001E-2</v>
@@ -9837,7 +9837,7 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="J28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K28">
         <v>1995</v>
@@ -9857,16 +9857,16 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E29">
         <v>5.8099999999999999E-2</v>
@@ -9884,7 +9884,7 @@
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="J29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K29">
         <v>1995</v>
@@ -9904,16 +9904,16 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30">
         <v>0.32800000000000001</v>
@@ -9931,7 +9931,7 @@
         <v>0.08</v>
       </c>
       <c r="J30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K30">
         <v>1995</v>
@@ -9951,16 +9951,16 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C31" t="s">
         <v>192</v>
       </c>
-      <c r="C31" t="s">
-        <v>193</v>
-      </c>
       <c r="D31" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E31">
         <v>2.3E-2</v>
@@ -9978,13 +9978,13 @@
       </c>
       <c r="I31" s="5"/>
       <c r="J31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K31">
         <v>1990</v>
       </c>
       <c r="L31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M31" s="14">
         <f t="shared" si="1"/>
@@ -10001,16 +10001,16 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E32">
         <v>2</v>
@@ -10026,7 +10026,7 @@
       </c>
       <c r="I32" s="5"/>
       <c r="J32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K32">
         <v>1990</v>
@@ -10046,16 +10046,16 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E33">
         <v>0.39</v>
@@ -10071,7 +10071,7 @@
       </c>
       <c r="I33" s="5"/>
       <c r="J33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K33">
         <v>1990</v>
@@ -10091,16 +10091,16 @@
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E34">
         <v>0.57499999999999996</v>
@@ -10115,7 +10115,7 @@
         <v>9.8700000000000003E-4</v>
       </c>
       <c r="J34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K34">
         <v>1990</v>
@@ -10135,16 +10135,16 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E35">
         <v>0.17</v>
@@ -10159,7 +10159,7 @@
         <v>1.6200000000000001E-4</v>
       </c>
       <c r="J35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K35">
         <v>1990</v>
@@ -10179,16 +10179,16 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C36" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E36">
         <v>2</v>
@@ -10203,7 +10203,7 @@
         <v>1.32E-2</v>
       </c>
       <c r="J36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K36">
         <v>1990</v>
@@ -10223,16 +10223,16 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C37" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E37">
         <v>0.61499999999999999</v>
@@ -10247,7 +10247,7 @@
         <v>1.25E-3</v>
       </c>
       <c r="J37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K37">
         <v>1990</v>
@@ -10267,16 +10267,16 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E38">
         <v>9.1999999999999998E-2</v>
@@ -10292,7 +10292,7 @@
         <v>2.2500000000000001E-5</v>
       </c>
       <c r="J38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K38">
         <v>1990</v>
@@ -10312,16 +10312,16 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C39" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E39">
         <v>5.3999999999999999E-2</v>
@@ -10337,7 +10337,7 @@
         <v>6.6599999999999998E-6</v>
       </c>
       <c r="J39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K39">
         <v>1990</v>
@@ -10357,16 +10357,16 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E40">
         <v>7.0000000000000001E-3</v>
@@ -10382,7 +10382,7 @@
         <v>2.5699999999999999E-7</v>
       </c>
       <c r="J40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K40">
         <v>1990</v>
@@ -10402,16 +10402,16 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E41">
         <v>6.0999999999999999E-2</v>
@@ -10427,7 +10427,7 @@
         <v>2.4499999999999999E-5</v>
       </c>
       <c r="J41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K41">
         <v>1990</v>
@@ -10447,16 +10447,16 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E42">
         <v>0.104</v>
@@ -10471,7 +10471,7 @@
         <v>5.9599999999999997E-6</v>
       </c>
       <c r="J42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K42">
         <v>1990</v>
@@ -10491,16 +10491,16 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D43" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E43">
         <v>0.08</v>
@@ -10515,7 +10515,7 @@
         <v>5.8699999999999997E-5</v>
       </c>
       <c r="J43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K43">
         <v>1990</v>
@@ -10535,16 +10535,16 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C44" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E44">
         <v>0.54</v>
@@ -10559,7 +10559,7 @@
         <v>1.01E-3</v>
       </c>
       <c r="J44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K44">
         <v>1990</v>
@@ -10579,16 +10579,16 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E45">
         <v>0.27</v>
@@ -10603,7 +10603,7 @@
         <v>4.6500000000000003E-4</v>
       </c>
       <c r="J45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K45">
         <v>1990</v>
@@ -10623,16 +10623,16 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E46">
         <v>0.34</v>
@@ -10647,7 +10647,7 @@
         <v>6.0700000000000001E-4</v>
       </c>
       <c r="J46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K46">
         <v>1990</v>
@@ -10667,16 +10667,16 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E47">
         <v>0.79</v>
@@ -10691,7 +10691,7 @@
         <v>3.0300000000000001E-3</v>
       </c>
       <c r="J47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K47">
         <v>1990</v>
@@ -10711,16 +10711,16 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E48">
         <v>0.4</v>
@@ -10735,13 +10735,13 @@
         <v>1.83E-4</v>
       </c>
       <c r="J48" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K48">
         <v>1968</v>
       </c>
       <c r="L48" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M48" s="14">
         <f>0.00194*E48^1.953</f>
@@ -10758,16 +10758,16 @@
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E49">
         <v>0.50739999999999996</v>
@@ -10779,13 +10779,13 @@
         <v>3.28E-4</v>
       </c>
       <c r="J49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K49">
         <v>2009</v>
       </c>
       <c r="L49" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M49" s="14">
         <f t="shared" si="1"/>
@@ -10802,16 +10802,16 @@
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>199</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" t="s">
         <v>201</v>
       </c>
-      <c r="C50" t="s">
-        <v>202</v>
-      </c>
       <c r="D50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E50">
         <v>8.7279999999999996E-2</v>
@@ -10823,13 +10823,13 @@
         <v>4.0200000000000001E-5</v>
       </c>
       <c r="J50" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K50">
         <v>2004</v>
       </c>
       <c r="L50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="M50" s="14">
         <f t="shared" si="1"/>
@@ -10846,16 +10846,16 @@
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E51">
         <v>0.2893</v>
@@ -10873,7 +10873,7 @@
         <v>3.4175999999999998E-4</v>
       </c>
       <c r="J51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K51">
         <v>2007</v>
@@ -10893,16 +10893,16 @@
     </row>
     <row r="52" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E52" s="10">
         <v>0.2893</v>
@@ -10916,7 +10916,7 @@
         <v>1.8799999999999999E-4</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K52" s="10">
         <v>2007</v>
@@ -10926,16 +10926,16 @@
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C53" t="s">
         <v>238</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>239</v>
-      </c>
-      <c r="D53" t="s">
-        <v>240</v>
       </c>
       <c r="E53">
         <v>3.46E-3</v>
@@ -10952,13 +10952,13 @@
         <v>1.7800000000000001E-8</v>
       </c>
       <c r="J53" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K53">
         <v>1993</v>
       </c>
       <c r="L53" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M53" s="14">
         <f t="shared" ref="M53:M61" si="4">0.00194*E53^1.953</f>
@@ -10975,16 +10975,16 @@
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>237</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C54" t="s">
         <v>238</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>239</v>
-      </c>
-      <c r="D54" t="s">
-        <v>240</v>
       </c>
       <c r="E54">
         <v>3.6600000000000001E-3</v>
@@ -11000,7 +11000,7 @@
         <v>1.8250000000000001E-8</v>
       </c>
       <c r="J54" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K54">
         <v>1993</v>
@@ -11020,16 +11020,16 @@
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>237</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C55" t="s">
         <v>238</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>239</v>
-      </c>
-      <c r="D55" t="s">
-        <v>240</v>
       </c>
       <c r="E55">
         <v>3.9300000000000003E-3</v>
@@ -11045,7 +11045,7 @@
         <v>2.4999999999999999E-8</v>
       </c>
       <c r="J55" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K55">
         <v>1993</v>
@@ -11065,16 +11065,16 @@
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>237</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C56" t="s">
         <v>238</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>239</v>
-      </c>
-      <c r="D56" t="s">
-        <v>240</v>
       </c>
       <c r="E56">
         <v>4.1000000000000003E-3</v>
@@ -11090,7 +11090,7 @@
         <v>2.955E-8</v>
       </c>
       <c r="J56" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K56">
         <v>1993</v>
@@ -11110,16 +11110,16 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>240</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="C57" t="s">
+        <v>238</v>
+      </c>
+      <c r="D57" t="s">
         <v>239</v>
-      </c>
-      <c r="D57" t="s">
-        <v>240</v>
       </c>
       <c r="E57">
         <v>4.2399999999999998E-3</v>
@@ -11135,7 +11135,7 @@
         <v>6.96E-9</v>
       </c>
       <c r="J57" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K57">
         <v>1993</v>
@@ -11155,16 +11155,16 @@
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>240</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="C58" t="s">
+        <v>238</v>
+      </c>
+      <c r="D58" t="s">
         <v>239</v>
-      </c>
-      <c r="D58" t="s">
-        <v>240</v>
       </c>
       <c r="E58">
         <v>4.2399999999999998E-3</v>
@@ -11180,7 +11180,7 @@
         <v>1.05E-8</v>
       </c>
       <c r="J58" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K58">
         <v>1993</v>
@@ -11200,16 +11200,16 @@
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>240</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="C59" t="s">
+        <v>238</v>
+      </c>
+      <c r="D59" t="s">
         <v>239</v>
-      </c>
-      <c r="D59" t="s">
-        <v>240</v>
       </c>
       <c r="E59">
         <v>4.1000000000000003E-3</v>
@@ -11225,7 +11225,7 @@
         <v>1.51E-8</v>
       </c>
       <c r="J59" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K59">
         <v>1993</v>
@@ -11245,16 +11245,16 @@
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>240</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>242</v>
-      </c>
       <c r="C60" t="s">
+        <v>238</v>
+      </c>
+      <c r="D60" t="s">
         <v>239</v>
-      </c>
-      <c r="D60" t="s">
-        <v>240</v>
       </c>
       <c r="E60">
         <v>4.5399999999999998E-3</v>
@@ -11270,7 +11270,7 @@
         <v>1.3799999999999999E-8</v>
       </c>
       <c r="J60" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K60">
         <v>1993</v>
@@ -11290,16 +11290,16 @@
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>254</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>256</v>
-      </c>
       <c r="C61" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E61">
         <v>0.35149999999999998</v>
@@ -11314,7 +11314,7 @@
         <v>7.4089000000000002E-4</v>
       </c>
       <c r="J61" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K61">
         <v>2015</v>
@@ -11379,152 +11379,152 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" t="s">
         <v>228</v>
       </c>
-      <c r="B2" t="s">
-        <v>229</v>
-      </c>
       <c r="C2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B3">
         <v>2007</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4">
         <v>2007</v>
       </c>
       <c r="C4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B5">
         <v>2009</v>
       </c>
       <c r="C5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8">
         <v>2015</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B9">
         <v>2010</v>
       </c>
       <c r="C9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B10">
         <v>2005</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" t="s">
         <v>250</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="7" t="s">
         <v>251</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" t="s">
         <v>253</v>
-      </c>
-      <c r="C12" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -11564,30 +11564,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B2">
         <v>2008</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -11614,27 +11614,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B1" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" t="s">
         <v>277</v>
       </c>
-      <c r="B1" t="s">
-        <v>276</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>278</v>
-      </c>
-      <c r="D1" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B2">
         <v>1100</v>
       </c>
       <c r="C2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D2">
         <v>1998</v>
@@ -11642,13 +11642,13 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>2060</v>
       </c>
       <c r="C3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D3">
         <v>2010</v>
@@ -11656,13 +11656,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B4">
         <v>1060</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D4">
         <v>2015</v>
@@ -11670,7 +11670,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B5">
         <v>660</v>
@@ -11678,7 +11678,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -11726,73 +11726,73 @@
   <sheetData>
     <row r="1" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>288</v>
-      </c>
       <c r="M1" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>267</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q1" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>270</v>
-      </c>
       <c r="R1" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="S1" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="T1" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="U1" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="V1" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="V1" s="17" t="s">
-        <v>266</v>
-      </c>
       <c r="W1" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -11830,12 +11830,12 @@
         <v>2.2338776875349999E-3</v>
       </c>
       <c r="W2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3">
         <v>1.0649999999999999</v>
@@ -11849,12 +11849,12 @@
         <v>2.3010000000000001E-4</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4">
         <v>3.96</v>
@@ -11862,7 +11862,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B5">
         <v>8.1500000000000003E-2</v>
@@ -11876,17 +11876,17 @@
         <v>1.8359999999999999E-4</v>
       </c>
       <c r="W5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -11900,7 +11900,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11914,34 +11914,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>289</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G1" t="s">
         <v>290</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>291</v>
       </c>
-      <c r="G1" t="s">
-        <v>292</v>
-      </c>
-      <c r="H1" t="s">
-        <v>293</v>
-      </c>
       <c r="I1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -11949,7 +11949,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1">
         <f>AVERAGE('[1] ImageJ'!F2:F4)</f>
@@ -11987,7 +11987,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="1">
         <f>AVERAGE('[1] ImageJ'!F90:F92)</f>
@@ -12025,7 +12025,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <f>AVERAGE('[1] ImageJ'!F180:F182)</f>
@@ -12063,7 +12063,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1">
         <f>AVERAGE('[1] ImageJ'!F267:F269)</f>
@@ -12101,7 +12101,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1">
         <f>AVERAGE('[1] ImageJ'!F357:F359)</f>
@@ -12139,7 +12139,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <f>AVERAGE('[1] ImageJ'!F438:F440)</f>
@@ -12177,7 +12177,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="1">
         <f>AVERAGE('[1] ImageJ'!F511:F513)</f>
@@ -12215,7 +12215,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1">
         <f>AVERAGE('[1] ImageJ'!F578:F580)</f>
@@ -12253,7 +12253,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
         <f>AVERAGE('[1] ImageJ'!F641:F643)</f>
@@ -12291,7 +12291,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="1">
         <f>AVERAGE('[1] ImageJ'!F699:F701)</f>
@@ -12330,7 +12330,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1">
         <f>AVERAGE('[1] ImageJ'!F756:F758)</f>
@@ -12368,7 +12368,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1">
         <f>AVERAGE('[1] ImageJ'!F805:F807)</f>
@@ -12406,7 +12406,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="1">
         <f>AVERAGE('[1] ImageJ'!F857:F859)</f>
@@ -12444,7 +12444,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="1">
         <f>AVERAGE([2]Sheet2!F908:F910)</f>
@@ -12482,7 +12482,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="1">
         <f>AVERAGE([2]Sheet2!F958:F960)</f>
@@ -12520,7 +12520,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="1">
         <f>AVERAGE([2]Sheet2!F1007:F1009)</f>
@@ -12558,7 +12558,7 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18" s="1">
         <f>AVERAGE([2]Sheet2!F1056:F1058)</f>
@@ -12596,7 +12596,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="1">
         <f>AVERAGE([2]Sheet2!F1102:F1104)</f>
@@ -12634,7 +12634,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="1">
         <f>AVERAGE([2]Sheet2!F1150:F1152)</f>
@@ -12672,7 +12672,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="1">
         <f>AVERAGE([2]Sheet2!F1200:F1202)</f>
@@ -12710,7 +12710,7 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
         <f>AVERAGE([2]Sheet2!F1250:F1252)</f>
@@ -12748,7 +12748,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1">
         <f>AVERAGE([2]Sheet2!F1301:F1303)</f>
@@ -12786,7 +12786,7 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="1">
         <v>4.1779999999999999</v>
@@ -12818,7 +12818,7 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="1">
         <v>4.1779999999999999</v>
@@ -12850,7 +12850,7 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="1">
         <v>4.1779999999999999</v>
@@ -12882,7 +12882,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="1">
         <v>4.1779999999999999</v>
@@ -12914,7 +12914,7 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="1">
         <v>4.1779999999999999</v>
@@ -12947,7 +12947,7 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="1">
         <v>4.1779999999999999</v>
@@ -12979,7 +12979,7 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1">
         <v>4.1779999999999999</v>
@@ -13011,7 +13011,7 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1">
         <v>4.1779999999999999</v>
@@ -13043,7 +13043,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1">
         <v>0</v>
@@ -13095,31 +13095,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E1" t="s">
         <v>294</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>295</v>
       </c>
-      <c r="E1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F1" t="s">
-        <v>297</v>
-      </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H1" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" t="s">
         <v>260</v>
-      </c>
-      <c r="I1" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -13127,7 +13127,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C2">
         <v>7.8399999999999997E-3</v>
@@ -13147,7 +13147,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>5.9100000000000003E-3</v>
@@ -13167,7 +13167,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>1.8699999999999999E-3</v>
@@ -13187,7 +13187,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5">
         <v>2.4299999999999999E-3</v>
@@ -13207,7 +13207,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6">
         <v>2.6200000000000003E-4</v>
@@ -13227,7 +13227,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C7">
         <v>1.7100000000000001E-4</v>
@@ -13247,7 +13247,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -13267,7 +13267,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -13287,7 +13287,7 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -13304,10 +13304,10 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11">
         <v>0.10349999999999999</v>
@@ -13315,10 +13315,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>0.13669999999999999</v>
@@ -13326,10 +13326,10 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13">
         <v>0.13669999999999999</v>
@@ -13337,10 +13337,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14">
         <v>6.1269999999999998E-2</v>
@@ -13348,42 +13348,42 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated referencing the issues raised in 2020-09-02 mathematicalfunctions feedback #3
</commit_message>
<xml_diff>
--- a/data/Master_AnatomicalData.xlsx
+++ b/data/Master_AnatomicalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE82F6DF-98AB-493B-A37D-A4BD6772F66D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BA1179-86A8-4710-8F6E-7EBBED6D235D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4500" yWindow="2055" windowWidth="21600" windowHeight="14655" tabRatio="823" activeTab="6" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="2535" yWindow="0" windowWidth="15135" windowHeight="15060" tabRatio="823" firstSheet="3" activeTab="7" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="303">
   <si>
     <t>Species</t>
   </si>
@@ -1109,7 +1109,7 @@
       <sheetName val="Final"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="F2">
@@ -5768,8 +5768,8 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11897,10 +11897,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA69E9DF-4385-4F68-B3FA-768F27E5E0EC}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13070,6 +13070,254 @@
         <v>6.225E-2</v>
       </c>
     </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>55</v>
+      </c>
+      <c r="B37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>55</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B47" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+      <c r="B49" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B52" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>55</v>
+      </c>
+      <c r="B59" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>55</v>
+      </c>
+      <c r="B62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13077,10 +13325,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B73562-5146-43F5-B742-9562EED8ED07}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13304,51 +13552,39 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="D11">
-        <v>0.10349999999999999</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
         <v>36</v>
       </c>
-      <c r="D12">
-        <v>0.13669999999999999</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="D13">
-        <v>0.13669999999999999</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B14" t="s">
         <v>37</v>
       </c>
-      <c r="D14">
-        <v>6.1269999999999998E-2</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>38</v>
@@ -13356,33 +13592,117 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>44</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>0.10349999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>0.13669999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22">
+        <v>0.13669999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>6.1269999999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating codes to calculate the head and neck CG and MOI
</commit_message>
<xml_diff>
--- a/data/Master_AnatomicalData.xlsx
+++ b/data/Master_AnatomicalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3BA1179-86A8-4710-8F6E-7EBBED6D235D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFD894D-7848-49EF-B98E-F8133332AD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="0" windowWidth="15135" windowHeight="15060" tabRatio="823" firstSheet="3" activeTab="7" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="-540" yWindow="75" windowWidth="21600" windowHeight="14970" tabRatio="823" firstSheet="3" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -19,12 +19,13 @@
     <sheet name="Existing material density data" sheetId="10" r:id="rId4"/>
     <sheet name="MaterialSpecs" sheetId="11" r:id="rId5"/>
     <sheet name="FullBird" sheetId="5" r:id="rId6"/>
-    <sheet name="Feathers" sheetId="1" r:id="rId7"/>
-    <sheet name="Bones" sheetId="2" r:id="rId8"/>
+    <sheet name="BodyPositioning" sheetId="12" r:id="rId7"/>
+    <sheet name="Feathers" sheetId="1" r:id="rId8"/>
+    <sheet name="Bones" sheetId="2" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,8 +44,123 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{083A40A9-3471-414E-BCDA-14E66DE7A0A5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgFQ
+tc={2C94B427-8DD5-604E-BFA6-D3362626B142}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    y-axis</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D3AE0056-5F5B-4BF7-A1F5-523799EB1945}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgFI
+tc={E6AA00D6-7290-8A40-813A-D95B0503F296}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from tip of beak back along body axis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EFB222FD-14CA-46F7-8B41-B36DE218B945}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgEw
+tc={F7284A37-F73A-694D-B6D7-DE828D679370}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from top of head towards the bottom</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{0A824F0A-AFF0-458F-9215-076D99A68DAB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgFE
+tc={277DF153-B7EE-7743-94B9-763AB873DADC}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from neck origin (clavicle) back along body axis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{003EB70D-6858-43D7-B346-409B39340F27}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgE8
+tc={8FFE6BE7-2A7A-6048-96C7-4034214EC84C}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from back towards stomach</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="318">
   <si>
     <t>Species</t>
   </si>
@@ -838,9 +954,6 @@
     <t>Cortical area</t>
   </si>
   <si>
-    <t>Body length (m)</t>
-  </si>
-  <si>
     <t>Body max width (m)</t>
   </si>
   <si>
@@ -853,21 +966,6 @@
     <t>x-loc of shoulder (m)</t>
   </si>
   <si>
-    <t>Mass of tail feathers (kg)</t>
-  </si>
-  <si>
-    <t>Mass of torso (kg)</t>
-  </si>
-  <si>
-    <t>Head CG rel to RH shoulder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torso CG relative to RH humeral head </t>
-  </si>
-  <si>
-    <t>Tail CG rel to RH shoulder</t>
-  </si>
-  <si>
     <t>Bennet</t>
   </si>
   <si>
@@ -913,12 +1011,6 @@
     <t>manus_skin_mass</t>
   </si>
   <si>
-    <t>head_mass</t>
-  </si>
-  <si>
-    <t>tail_mass</t>
-  </si>
-  <si>
     <t>l_cal</t>
   </si>
   <si>
@@ -962,6 +1054,75 @@
   </si>
   <si>
     <t>w_cal</t>
+  </si>
+  <si>
+    <t>cya_ste</t>
+  </si>
+  <si>
+    <t>head_mass_kg</t>
+  </si>
+  <si>
+    <t>head_length_m</t>
+  </si>
+  <si>
+    <t>head_height_m</t>
+  </si>
+  <si>
+    <t>neck_length_m</t>
+  </si>
+  <si>
+    <t>neck_width_m</t>
+  </si>
+  <si>
+    <t>neck_mass_kg</t>
+  </si>
+  <si>
+    <t>head_torsotail_mass_kg</t>
+  </si>
+  <si>
+    <t>x_loc_HeadCoG_m</t>
+  </si>
+  <si>
+    <t>z_loc_HeadCoG_m</t>
+  </si>
+  <si>
+    <t>x_loc_TorsotailCoG_m</t>
+  </si>
+  <si>
+    <t>z_loc_TorsotailCoG_m</t>
+  </si>
+  <si>
+    <t>left_leg_mass_kg</t>
+  </si>
+  <si>
+    <t>right_leg_mass_kg</t>
+  </si>
+  <si>
+    <t>torsotail_length_m</t>
+  </si>
+  <si>
+    <t>x_loc_of_body_max_cm</t>
+  </si>
+  <si>
+    <t>x_loc_of_humeral_insert_cm</t>
+  </si>
+  <si>
+    <t>y_loc_of_humeral_insert_cm</t>
+  </si>
+  <si>
+    <t>z_loc_of_humeral_insert_cm</t>
+  </si>
+  <si>
+    <t>x_loc_leg_insertion_cm</t>
+  </si>
+  <si>
+    <t>body_width_at_leg_insert_m</t>
+  </si>
+  <si>
+    <t>body_width_max_m</t>
+  </si>
+  <si>
+    <t>body_height_max_m</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1002,6 +1163,37 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1037,7 +1229,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1070,6 +1262,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11614,16 +11810,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="C1" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D1" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11634,7 +11830,7 @@
         <v>1100</v>
       </c>
       <c r="C2" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D2">
         <v>1998</v>
@@ -11648,7 +11844,7 @@
         <v>2060</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D3">
         <v>2010</v>
@@ -11670,7 +11866,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B5">
         <v>660</v>
@@ -11678,7 +11874,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -11690,14 +11886,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBCFE0-47B2-4031-92B0-C1E328A3FA99}">
-  <dimension ref="A1:W7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBCFE0-47B2-4031-92B0-C1E328A3FA99}">
+  <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
+      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11709,93 +11905,112 @@
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="16.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" customWidth="1"/>
-    <col min="21" max="21" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19" customWidth="1"/>
-    <col min="23" max="23" width="68.7109375" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="16.5703125" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19" customWidth="1"/>
+    <col min="28" max="28" width="68.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>283</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="K1" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="L1" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="M1" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="N1" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="O1" s="21" t="s">
+        <v>309</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>297</v>
       </c>
-      <c r="H1" s="6" t="s">
-        <v>284</v>
-      </c>
-      <c r="I1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>298</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>307</v>
+      </c>
+      <c r="X1" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="S1" s="17" t="s">
+      <c r="Y1" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="Z1" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="U1" s="17" t="s">
+      <c r="AA1" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="V1" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="W1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -11829,11 +12044,11 @@
       <c r="J2">
         <v>2.2338776875349999E-3</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AB2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -11848,11 +12063,11 @@
         <f>D3*(12.8-1)</f>
         <v>2.3010000000000001E-4</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -11860,7 +12075,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -11875,32 +12090,214 @@
         <f>D5*(7.8-1)</f>
         <v>1.8359999999999999E-4</v>
       </c>
-      <c r="W5" t="s">
+      <c r="AB5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8">
+        <f>145.21/1000</f>
+        <v>0.14521000000000001</v>
+      </c>
+      <c r="C8">
+        <f>7.32/100</f>
+        <v>7.3200000000000001E-2</v>
+      </c>
+      <c r="K8">
+        <f>120.25/1000</f>
+        <v>0.12025</v>
+      </c>
+      <c r="L8" s="20">
+        <f>2.84/100</f>
+        <v>2.8399999999999998E-2</v>
+      </c>
+      <c r="M8" s="20">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="N8" s="20">
+        <f>4.2/100</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="O8">
+        <f>23.1/100</f>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="P8">
+        <f>6.76/100</f>
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="Q8">
+        <f>2.59/100</f>
+        <v>2.5899999999999999E-2</v>
+      </c>
+      <c r="R8">
+        <f>16.56/1000</f>
+        <v>1.6559999999999998E-2</v>
+      </c>
+      <c r="S8" s="18">
+        <f>4/100</f>
+        <v>0.04</v>
+      </c>
+      <c r="T8" s="18">
+        <f>0.85/100</f>
+        <v>8.5000000000000006E-3</v>
+      </c>
+      <c r="U8" s="18">
+        <f>7.29/1000</f>
+        <v>7.2899999999999996E-3</v>
+      </c>
+      <c r="V8" s="20">
+        <f>11.53/1000</f>
+        <v>1.1529999999999999E-2</v>
+      </c>
+      <c r="W8" s="20">
+        <f>11.49/1000</f>
+        <v>1.149E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBB0CD1-52C0-49A8-A7A1-8F0A98CC1A9A}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>295</v>
+      </c>
+      <c r="B8" s="20">
+        <v>4.4500000000000005E-2</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1.26E-2</v>
+      </c>
+      <c r="D8" s="20">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="F8" s="20">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="G8" s="20">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="H8" s="20">
+        <v>6.5000000000000006E-3</v>
+      </c>
+      <c r="I8" s="20">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="J8" s="20">
+        <v>5.3899999999999997E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA69E9DF-4385-4F68-B3FA-768F27E5E0EC}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11917,31 +12314,31 @@
         <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="C1" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D1" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="G1" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="H1" t="s">
+        <v>283</v>
+      </c>
+      <c r="I1" t="s">
         <v>291</v>
       </c>
-      <c r="I1" t="s">
-        <v>299</v>
-      </c>
       <c r="J1" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13323,12 +13720,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B73562-5146-43F5-B742-9562EED8ED07}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13346,19 +13743,19 @@
         <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="C1" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="D1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="G1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
completed including the torso/tail MOI and CG calculations - still need to add one more constraint on the optimization
</commit_message>
<xml_diff>
--- a/data/Master_AnatomicalData.xlsx
+++ b/data/Master_AnatomicalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDFD894D-7848-49EF-B98E-F8133332AD48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45DFD25-DE23-494C-9D59-6520F232F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-540" yWindow="75" windowWidth="21600" windowHeight="14970" tabRatio="823" firstSheet="3" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="-540" yWindow="75" windowWidth="21600" windowHeight="14970" tabRatio="823" firstSheet="4" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -66,6 +66,82 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     y-axis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X1" authorId="0" shapeId="0" xr:uid="{5CB3DAD5-CB45-4565-A09A-2098EB522C6A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgFI
+tc={E6AA00D6-7290-8A40-813A-D95B0503F296}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from tip of beak back along body axis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y1" authorId="0" shapeId="0" xr:uid="{3B240FBB-C5C4-46C4-99F5-43021824F47A}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgEw
+tc={F7284A37-F73A-694D-B6D7-DE828D679370}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from top of head towards the bottom</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z1" authorId="0" shapeId="0" xr:uid="{8295B6A5-413D-4295-A7AA-A2CA6760F855}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgFE
+tc={277DF153-B7EE-7743-94B9-763AB873DADC}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from neck origin (clavicle) back along body axis</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{09DB28DE-89AD-46F3-ABCE-D1FA78AF5BA1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="12"/>
+            <color theme="1"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>======
+ID#AAAAKdQCgE8
+tc={8FFE6BE7-2A7A-6048-96C7-4034214EC84C}    (2020-10-06 19:09:23)
+[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    measured from back towards stomach</t>
         </r>
       </text>
     </comment>
@@ -160,7 +236,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="314">
   <si>
     <t>Species</t>
   </si>
@@ -954,18 +1030,6 @@
     <t>Cortical area</t>
   </si>
   <si>
-    <t>Body max width (m)</t>
-  </si>
-  <si>
-    <t>Body max height (m)</t>
-  </si>
-  <si>
-    <t>x-loc of max body (m)</t>
-  </si>
-  <si>
-    <t>x-loc of shoulder (m)</t>
-  </si>
-  <si>
     <t>Bennet</t>
   </si>
   <si>
@@ -1104,18 +1168,6 @@
     <t>x_loc_of_body_max_cm</t>
   </si>
   <si>
-    <t>x_loc_of_humeral_insert_cm</t>
-  </si>
-  <si>
-    <t>y_loc_of_humeral_insert_cm</t>
-  </si>
-  <si>
-    <t>z_loc_of_humeral_insert_cm</t>
-  </si>
-  <si>
-    <t>x_loc_leg_insertion_cm</t>
-  </si>
-  <si>
     <t>body_width_at_leg_insert_m</t>
   </si>
   <si>
@@ -1123,6 +1175,18 @@
   </si>
   <si>
     <t>body_height_max_m</t>
+  </si>
+  <si>
+    <t>x_loc_leg_insertion_m</t>
+  </si>
+  <si>
+    <t>z_loc_of_humeral_insert_m</t>
+  </si>
+  <si>
+    <t>y_loc_of_humeral_insert_m</t>
+  </si>
+  <si>
+    <t>x_loc_of_humeral_insert_m</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1260,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1206,12 +1270,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1229,7 +1287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1261,7 +1319,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -11810,16 +11867,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11830,7 +11887,7 @@
         <v>1100</v>
       </c>
       <c r="C2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D2">
         <v>1998</v>
@@ -11844,7 +11901,7 @@
         <v>2060</v>
       </c>
       <c r="C3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D3">
         <v>2010</v>
@@ -11866,7 +11923,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B5">
         <v>660</v>
@@ -11874,7 +11931,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B6">
         <v>37</v>
@@ -11887,13 +11944,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBCFE0-47B2-4031-92B0-C1E328A3FA99}">
-  <dimension ref="A1:AB8"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11917,100 +11974,119 @@
     <col min="19" max="21" width="16.5703125" customWidth="1"/>
     <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19" customWidth="1"/>
-    <col min="28" max="28" width="68.7109375" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="68.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="I1" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="K1" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="S1" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="T1" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="U1" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="V1" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="W1" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="X1" s="20" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y1" s="20" t="s">
+        <v>300</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="AA1" s="20" t="s">
         <v>302</v>
       </c>
-      <c r="L1" s="21" t="s">
-        <v>316</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>315</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>317</v>
-      </c>
-      <c r="O1" s="21" t="s">
-        <v>309</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="S1" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="T1" s="21" t="s">
-        <v>300</v>
-      </c>
-      <c r="U1" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="V1" s="21" t="s">
-        <v>308</v>
-      </c>
-      <c r="W1" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="X1" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="Y1" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="Z1" s="17" t="s">
-        <v>263</v>
-      </c>
-      <c r="AA1" s="17" t="s">
-        <v>264</v>
-      </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="20" t="s">
+        <v>306</v>
+      </c>
+      <c r="AC1" s="20" t="s">
+        <v>313</v>
+      </c>
+      <c r="AD1" s="20" t="s">
+        <v>312</v>
+      </c>
+      <c r="AE1" s="20" t="s">
+        <v>311</v>
+      </c>
+      <c r="AF1" s="20" t="s">
+        <v>310</v>
+      </c>
+      <c r="AG1" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12044,11 +12120,11 @@
       <c r="J2">
         <v>2.2338776875349999E-3</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AG2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -12063,11 +12139,11 @@
         <f>D3*(12.8-1)</f>
         <v>2.3010000000000001E-4</v>
       </c>
-      <c r="AB3" s="2" t="s">
+      <c r="AG3" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -12075,7 +12151,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -12090,23 +12166,23 @@
         <f>D5*(7.8-1)</f>
         <v>1.8359999999999999E-4</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AG5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B8">
         <f>145.21/1000</f>
@@ -12120,14 +12196,14 @@
         <f>120.25/1000</f>
         <v>0.12025</v>
       </c>
-      <c r="L8" s="20">
+      <c r="L8" s="19">
         <f>2.84/100</f>
         <v>2.8399999999999998E-2</v>
       </c>
-      <c r="M8" s="20">
+      <c r="M8" s="19">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="N8" s="20">
+      <c r="N8" s="19">
         <f>4.2/100</f>
         <v>4.2000000000000003E-2</v>
       </c>
@@ -12147,25 +12223,52 @@
         <f>16.56/1000</f>
         <v>1.6559999999999998E-2</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="17">
         <f>4/100</f>
         <v>0.04</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="17">
         <f>0.85/100</f>
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="17">
         <f>7.29/1000</f>
         <v>7.2899999999999996E-3</v>
       </c>
-      <c r="V8" s="20">
+      <c r="V8" s="19">
         <f>11.53/1000</f>
         <v>1.1529999999999999E-2</v>
       </c>
-      <c r="W8" s="20">
+      <c r="W8" s="19">
         <f>11.49/1000</f>
         <v>1.149E-2</v>
+      </c>
+      <c r="X8" s="19">
+        <v>4.4500000000000005E-2</v>
+      </c>
+      <c r="Y8" s="19">
+        <v>1.26E-2</v>
+      </c>
+      <c r="Z8" s="19">
+        <v>5.3699999999999998E-2</v>
+      </c>
+      <c r="AA8" s="19">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="AB8" s="19">
+        <v>3.9399999999999998E-2</v>
+      </c>
+      <c r="AC8" s="19">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="AD8" s="19">
+        <v>6.5000000000000006E-3</v>
+      </c>
+      <c r="AE8" s="19">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="AF8" s="19">
+        <v>5.3899999999999997E-2</v>
       </c>
     </row>
   </sheetData>
@@ -12179,8 +12282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBB0CD1-52C0-49A8-A7A1-8F0A98CC1A9A}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12196,32 +12299,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="E1" s="19" t="s">
+      <c r="B1" s="18" t="s">
+        <v>299</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>300</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>301</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" s="19" t="s">
         <v>310</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>312</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="J1" s="20" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -12256,33 +12359,33 @@
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>295</v>
-      </c>
-      <c r="B8" s="20">
+        <v>291</v>
+      </c>
+      <c r="B8" s="19">
         <v>4.4500000000000005E-2</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="19">
         <v>1.26E-2</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="19">
         <v>5.3699999999999998E-2</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="19">
         <v>1.3999999999999999E-2</v>
       </c>
-      <c r="F8" s="20">
+      <c r="F8" s="19">
         <v>3.9399999999999998E-2</v>
       </c>
-      <c r="G8" s="20">
+      <c r="G8" s="19">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="19">
         <v>6.5000000000000006E-3</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="19">
         <v>6.9999999999999993E-3</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="19">
         <v>5.3899999999999997E-2</v>
       </c>
     </row>
@@ -12314,31 +12417,31 @@
         <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="D1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="G1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="I1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="J1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13725,7 +13828,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E12" sqref="E12:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13743,19 +13846,19 @@
         <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="F1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="G1" t="s">
         <v>47</v>

</xml_diff>

<commit_message>
full calculation of bird results complete. May still need to add tail separately later
</commit_message>
<xml_diff>
--- a/data/Master_AnatomicalData.xlsx
+++ b/data/Master_AnatomicalData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Inman PC\Documents\birdmoment\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45DFD25-DE23-494C-9D59-6520F232F5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0166DDC-9337-4B01-86F0-32E817C477B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-540" yWindow="75" windowWidth="21600" windowHeight="14970" tabRatio="823" firstSheet="4" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
+    <workbookView xWindow="7305" yWindow="1260" windowWidth="21600" windowHeight="14970" tabRatio="823" firstSheet="4" activeTab="5" xr2:uid="{7BBA85BD-A929-4F3F-9778-E1081C0BF18C}"/>
   </bookViews>
   <sheets>
     <sheet name="Tracking" sheetId="7" r:id="rId1"/>
@@ -19,15 +19,15 @@
     <sheet name="Existing material density data" sheetId="10" r:id="rId4"/>
     <sheet name="MaterialSpecs" sheetId="11" r:id="rId5"/>
     <sheet name="FullBird" sheetId="5" r:id="rId6"/>
-    <sheet name="BodyPositioning" sheetId="12" r:id="rId7"/>
-    <sheet name="Feathers" sheetId="1" r:id="rId8"/>
-    <sheet name="Bones" sheetId="2" r:id="rId9"/>
+    <sheet name="Feathers" sheetId="1" r:id="rId7"/>
+    <sheet name="Bones" sheetId="2" r:id="rId8"/>
   </sheets>
   <externalReferences>
+    <externalReference r:id="rId9"/>
     <externalReference r:id="rId10"/>
-    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -149,94 +149,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{D3AE0056-5F5B-4BF7-A1F5-523799EB1945}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAKdQCgFI
-tc={E6AA00D6-7290-8A40-813A-D95B0503F296}    (2020-10-06 19:09:23)
-[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    measured from tip of beak back along body axis</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{EFB222FD-14CA-46F7-8B41-B36DE218B945}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAKdQCgEw
-tc={F7284A37-F73A-694D-B6D7-DE828D679370}    (2020-10-06 19:09:23)
-[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    measured from top of head towards the bottom</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{0A824F0A-AFF0-458F-9215-076D99A68DAB}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAKdQCgFE
-tc={277DF153-B7EE-7743-94B9-763AB873DADC}    (2020-10-06 19:09:23)
-[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    measured from neck origin (clavicle) back along body axis</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{003EB70D-6858-43D7-B346-409B39340F27}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="12"/>
-            <color theme="1"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-          </rPr>
-          <t>======
-ID#AAAAKdQCgE8
-tc={8FFE6BE7-2A7A-6048-96C7-4034214EC84C}    (2020-10-06 19:09:23)
-[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    measured from back towards stomach</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="314">
   <si>
     <t>Species</t>
   </si>
@@ -1072,9 +986,6 @@
     <t>manus_muscle_mass</t>
   </si>
   <si>
-    <t>manus_skin_mass</t>
-  </si>
-  <si>
     <t>l_cal</t>
   </si>
   <si>
@@ -1105,9 +1016,6 @@
     <t>antebrachial_muscle_mass</t>
   </si>
   <si>
-    <t>propatagiale_skin_mass</t>
-  </si>
-  <si>
     <t>l_f</t>
   </si>
   <si>
@@ -1141,9 +1049,6 @@
     <t>neck_mass_kg</t>
   </si>
   <si>
-    <t>head_torsotail_mass_kg</t>
-  </si>
-  <si>
     <t>x_loc_HeadCoG_m</t>
   </si>
   <si>
@@ -1165,9 +1070,6 @@
     <t>torsotail_length_m</t>
   </si>
   <si>
-    <t>x_loc_of_body_max_cm</t>
-  </si>
-  <si>
     <t>body_width_at_leg_insert_m</t>
   </si>
   <si>
@@ -1187,6 +1089,18 @@
   </si>
   <si>
     <t>x_loc_of_humeral_insert_m</t>
+  </si>
+  <si>
+    <t>x_loc_of_body_max_m</t>
+  </si>
+  <si>
+    <t>tertiary_mass</t>
+  </si>
+  <si>
+    <t>all_skin_coverts_mass</t>
+  </si>
+  <si>
+    <t>torsotail_mass_kg</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1232,13 +1146,6 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1287,7 +1194,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1321,8 +1228,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -11856,7 +11762,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B2" sqref="B1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11947,10 +11853,10 @@
   <dimension ref="A1:AG8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AD2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X4" sqref="X4"/>
+      <selection pane="bottomRight" activeCell="AE2" sqref="AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11963,8 +11869,7 @@
     <col min="7" max="7" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
@@ -12005,88 +11910,88 @@
         <v>273</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>274</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>286</v>
+        <v>311</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>275</v>
+        <v>312</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="S1" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="T1" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="U1" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="V1" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="W1" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="Z1" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="AA1" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="AB1" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD1" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="AE1" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="N1" s="20" t="s">
-        <v>309</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>305</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="S1" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="T1" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="U1" s="20" t="s">
-        <v>297</v>
-      </c>
-      <c r="V1" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="W1" s="20" t="s">
-        <v>303</v>
-      </c>
-      <c r="X1" s="20" t="s">
-        <v>299</v>
-      </c>
-      <c r="Y1" s="20" t="s">
-        <v>300</v>
-      </c>
-      <c r="Z1" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="AA1" s="20" t="s">
-        <v>302</v>
-      </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AF1" s="19" t="s">
         <v>306</v>
-      </c>
-      <c r="AC1" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="AD1" s="20" t="s">
-        <v>312</v>
-      </c>
-      <c r="AE1" s="20" t="s">
-        <v>311</v>
-      </c>
-      <c r="AF1" s="20" t="s">
-        <v>310</v>
       </c>
       <c r="AG1" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -12120,6 +12025,72 @@
       <c r="J2">
         <v>2.2338776875349999E-3</v>
       </c>
+      <c r="K2">
+        <v>0.87778</v>
+      </c>
+      <c r="L2" s="18">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="M2" s="18">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="N2" s="18">
+        <v>0.09</v>
+      </c>
+      <c r="O2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="P2">
+        <v>0.113</v>
+      </c>
+      <c r="Q2">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="R2">
+        <v>6.1240000000000001E-3</v>
+      </c>
+      <c r="S2" s="17">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="T2" s="17">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="U2" s="17">
+        <v>8.5800000000000001E-2</v>
+      </c>
+      <c r="V2" s="18">
+        <v>5.355E-2</v>
+      </c>
+      <c r="W2" s="18">
+        <v>5.5199999999999999E-2</v>
+      </c>
+      <c r="X2" s="18">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="Y2" s="18">
+        <v>2.4E-2</v>
+      </c>
+      <c r="Z2" s="18">
+        <v>0.109</v>
+      </c>
+      <c r="AA2" s="18">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AB2" s="18">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="AC2" s="18">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AD2" s="18">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AE2" s="18">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AF2" s="18">
+        <v>0.13800000000000001</v>
+      </c>
       <c r="AG2" t="s">
         <v>48</v>
       </c>
@@ -12182,7 +12153,7 @@
     </row>
     <row r="8" spans="1:33" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B8">
         <f>145.21/1000</f>
@@ -12193,17 +12164,17 @@
         <v>7.3200000000000001E-2</v>
       </c>
       <c r="K8">
-        <f>120.25/1000</f>
-        <v>0.12025</v>
-      </c>
-      <c r="L8" s="19">
+        <f>91.89/1000</f>
+        <v>9.1889999999999999E-2</v>
+      </c>
+      <c r="L8" s="18">
         <f>2.84/100</f>
         <v>2.8399999999999998E-2</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="18">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="N8" s="19">
+      <c r="N8" s="18">
         <f>4.2/100</f>
         <v>4.2000000000000003E-2</v>
       </c>
@@ -12235,39 +12206,39 @@
         <f>7.29/1000</f>
         <v>7.2899999999999996E-3</v>
       </c>
-      <c r="V8" s="19">
+      <c r="V8" s="18">
         <f>11.53/1000</f>
         <v>1.1529999999999999E-2</v>
       </c>
-      <c r="W8" s="19">
+      <c r="W8" s="18">
         <f>11.49/1000</f>
         <v>1.149E-2</v>
       </c>
-      <c r="X8" s="19">
+      <c r="X8" s="18">
         <v>4.4500000000000005E-2</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8" s="18">
         <v>1.26E-2</v>
       </c>
-      <c r="Z8" s="19">
+      <c r="Z8" s="18">
         <v>5.3699999999999998E-2</v>
       </c>
-      <c r="AA8" s="19">
-        <v>1.3999999999999999E-2</v>
-      </c>
-      <c r="AB8" s="19">
+      <c r="AA8" s="18">
+        <v>1.4E-2</v>
+      </c>
+      <c r="AB8" s="18">
         <v>3.9399999999999998E-2</v>
       </c>
-      <c r="AC8" s="19">
+      <c r="AC8" s="18">
         <v>9.4999999999999998E-3</v>
       </c>
-      <c r="AD8" s="19">
+      <c r="AD8" s="18">
         <v>6.5000000000000006E-3</v>
       </c>
-      <c r="AE8" s="19">
+      <c r="AE8" s="18">
         <v>6.9999999999999993E-3</v>
       </c>
-      <c r="AF8" s="19">
+      <c r="AF8" s="18">
         <v>5.3899999999999997E-2</v>
       </c>
     </row>
@@ -12279,123 +12250,6 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EBB0CD1-52C0-49A8-A7A1-8F0A98CC1A9A}">
-  <dimension ref="A1:J8"/>
-  <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
-        <v>299</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>300</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>301</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>312</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>291</v>
-      </c>
-      <c r="B8" s="19">
-        <v>4.4500000000000005E-2</v>
-      </c>
-      <c r="C8" s="19">
-        <v>1.26E-2</v>
-      </c>
-      <c r="D8" s="19">
-        <v>5.3699999999999998E-2</v>
-      </c>
-      <c r="E8" s="19">
-        <v>1.3999999999999999E-2</v>
-      </c>
-      <c r="F8" s="19">
-        <v>3.9399999999999998E-2</v>
-      </c>
-      <c r="G8" s="19">
-        <v>9.4999999999999998E-3</v>
-      </c>
-      <c r="H8" s="19">
-        <v>6.5000000000000006E-3</v>
-      </c>
-      <c r="I8" s="19">
-        <v>6.9999999999999993E-3</v>
-      </c>
-      <c r="J8" s="19">
-        <v>5.3899999999999997E-2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA69E9DF-4385-4F68-B3FA-768F27E5E0EC}">
   <dimension ref="A1:J63"/>
   <sheetViews>
@@ -12417,31 +12271,31 @@
         <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" t="s">
         <v>276</v>
-      </c>
-      <c r="D1" t="s">
-        <v>277</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G1" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" t="s">
         <v>278</v>
       </c>
-      <c r="H1" t="s">
-        <v>279</v>
-      </c>
       <c r="I1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="J1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -13823,7 +13677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B73562-5146-43F5-B742-9562EED8ED07}">
   <dimension ref="A1:I28"/>
   <sheetViews>
@@ -13846,19 +13700,19 @@
         <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D1" t="s">
         <v>280</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>281</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>282</v>
-      </c>
-      <c r="F1" t="s">
-        <v>283</v>
       </c>
       <c r="G1" t="s">
         <v>47</v>

</xml_diff>